<commit_message>
modify results, add log parsing script
</commit_message>
<xml_diff>
--- a/pa4/results/results.xlsx
+++ b/pa4/results/results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="25">
   <si>
     <t xml:space="preserve">tech</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">s-cc</t>
   </si>
   <si>
+    <t xml:space="preserve">We set up our logging system incorrectly so we only obtained one set of data for each setting. This requires re-work.</t>
+  </si>
+  <si>
     <t xml:space="preserve">min_msg_error_prcnt</t>
   </si>
   <si>
@@ -134,10 +137,12 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,12 +187,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,8 +293,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,7 +326,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>11</v>
@@ -331,7 +340,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>16</v>
@@ -351,10 +360,19 @@
       <c r="G2" s="0" t="n">
         <v>256</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <v>0.115999937057495</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.127251801490784</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0.185500144958496</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
@@ -375,10 +393,19 @@
         <f aca="false">G2/2</f>
         <v>128</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <v>0.119859933853149</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.151910791397095</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.292220115661621</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -399,10 +426,19 @@
         <f aca="false">G3/2</f>
         <v>64</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <v>0.184430122375488</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.266410012245178</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.436929941177368</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>16</v>
@@ -423,10 +459,19 @@
         <f aca="false">G4/2</f>
         <v>32</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <v>0.031110048294067</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.053247013092041</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.080209970474243</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -447,10 +492,19 @@
         <f aca="false">G5/2</f>
         <v>16</v>
       </c>
+      <c r="H6" s="0" t="n">
+        <v>0.031630039215088</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.054191813468933</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.111800193786621</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>16</v>
@@ -471,10 +525,19 @@
         <f aca="false">G6/2</f>
         <v>8</v>
       </c>
+      <c r="H7" s="0" t="n">
+        <v>0.03154993057251</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.469942407608032</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1.55883979797363</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>16</v>
@@ -495,10 +558,19 @@
         <f aca="false">G7/2</f>
         <v>4</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <v>0.03138017654419</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.312533802986145</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.833319902420044</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>16</v>
@@ -519,10 +591,19 @@
         <f aca="false">G8/2</f>
         <v>2</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <v>0.031509876251221</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.915821008682251</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>3.57241988182068</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>16</v>
@@ -542,6 +623,15 @@
       <c r="G10" s="0" t="n">
         <f aca="false">G9/2</f>
         <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.03137993812561</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.87031219959259</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>2.42447996139526</v>
       </c>
     </row>
   </sheetData>
@@ -672,13 +762,14 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.53"/>
   </cols>
@@ -712,7 +803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -728,8 +819,17 @@
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0" t="n">
+        <v>2.72663998603821</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3.15931596755981</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3.42025995254517</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
@@ -746,8 +846,17 @@
         <f aca="false">F2*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <v>2.92198991775513</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3.19700598716736</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>3.40961003303528</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
@@ -764,8 +873,17 @@
         <f aca="false">F3*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>2.93292999267578</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3.19725193977356</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3.39891982078552</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -782,8 +900,17 @@
         <f aca="false">F4*2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>2.94371008872986</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>3.22536206245422</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>3.42499017715454</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
@@ -800,8 +927,17 @@
         <f aca="false">F5*2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>2.95337009429932</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3.25001602172852</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3.5100200176239</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
@@ -818,8 +954,17 @@
         <f aca="false">F6*2</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>2.96954011917114</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>3.25627207756042</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>3.49545001983643</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -836,8 +981,17 @@
         <f aca="false">F7*2</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="n">
+        <v>2.9697802066803</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>3.25201992988586</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>3.48196983337402</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
@@ -854,8 +1008,17 @@
         <f aca="false">F8*2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="n">
+        <v>2.9515700340271</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>3.24429001808166</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>3.46737003326416</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
@@ -872,8 +1035,17 @@
         <f aca="false">F9*2</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="n">
+        <v>2.96009993553162</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>3.2562159538269</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>3.4640998840332</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
@@ -890,8 +1062,17 @@
         <f aca="false">F10*2</f>
         <v>512</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="n">
+        <v>2.96124005317688</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>3.27220406532288</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>3.5650999546051</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>14</v>
       </c>
@@ -908,8 +1089,17 @@
         <f aca="false">F11*2</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <v>3.01238012313843</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>3.30914597511291</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>3.66827988624573</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>14</v>
       </c>
@@ -926,6 +1116,15 @@
         <f aca="false">F12*2</f>
         <v>2048</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>3.01260018348694</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>3.33138003349304</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>3.7720000743866</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
@@ -944,8 +1143,17 @@
         <f aca="false">F13*2</f>
         <v>4096</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="n">
+        <v>3.02646994590759</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>3.34660801887512</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>3.85009002685547</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>14</v>
       </c>
@@ -962,8 +1170,17 @@
         <f aca="false">F14*2</f>
         <v>8192</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="0" t="n">
+        <v>2.95156979560852</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>3.32480797767639</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>3.84724998474121</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>14</v>
       </c>
@@ -980,8 +1197,17 @@
         <f aca="false">F15*2</f>
         <v>16384</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>2.89349007606506</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>3.3299699306488</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>3.9238498210907</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>14</v>
       </c>
@@ -998,8 +1224,17 @@
         <f aca="false">F16*2</f>
         <v>32768</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>2.9668300151825</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3.21306796073914</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>3.73062992095947</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>14</v>
       </c>
@@ -1016,8 +1251,17 @@
         <f aca="false">F17*2</f>
         <v>65536</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>3.01831007003784</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>3.28513398170471</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>3.81388998031616</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>14</v>
       </c>
@@ -1034,8 +1278,17 @@
         <f aca="false">F18*2</f>
         <v>131072</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>2.92688012123108</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>3.17299394607544</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>3.68725991249084</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>14</v>
       </c>
@@ -1052,8 +1305,17 @@
         <f aca="false">F19*2</f>
         <v>262144</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>2.7347400188446</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3.03940205574036</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>3.6664400100708</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>14</v>
       </c>
@@ -1070,8 +1332,17 @@
         <f aca="false">F20*2</f>
         <v>524288</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>2.36027979850769</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>2.66482796669006</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>3.30631995201111</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>16</v>
       </c>
@@ -1108,8 +1379,17 @@
       <c r="F23" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="n">
+        <v>4.28154993057251</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>3.92372798919678</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>4.28154993057251</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>16</v>
       </c>
@@ -1126,8 +1406,17 @@
         <f aca="false">F23*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="0" t="n">
+        <v>4.2696099281311</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>3.88751797676086</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>4.2696099281311</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>16</v>
       </c>
@@ -1144,8 +1433,17 @@
         <f aca="false">F24*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="0" t="n">
+        <v>4.22568988800049</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>3.85730991363525</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>4.22568988800049</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>16</v>
       </c>
@@ -1162,8 +1460,17 @@
         <f aca="false">F25*2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="n">
+        <v>4.18071007728577</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>3.82647399902344</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>4.18071007728577</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>16</v>
       </c>
@@ -1180,8 +1487,17 @@
         <f aca="false">F26*2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="0" t="n">
+        <v>4.14104008674622</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>3.80216403007507</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>4.14104008674622</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>16</v>
       </c>
@@ -1198,8 +1514,17 @@
         <f aca="false">F27*2</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="0" t="n">
+        <v>4.0946900844574</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>3.7696900844574</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>4.0946900844574</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>16</v>
       </c>
@@ -1216,8 +1541,17 @@
         <f aca="false">F28*2</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="0" t="n">
+        <v>4.04958987236023</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>3.73938794136047</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>4.04958987236023</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>16</v>
       </c>
@@ -1234,8 +1568,17 @@
         <f aca="false">F29*2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="n">
+        <v>4.00826001167297</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>3.70555801391602</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>4.00826001167297</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>16</v>
       </c>
@@ -1252,8 +1595,17 @@
         <f aca="false">F30*2</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="0" t="n">
+        <v>3.96534013748169</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>3.68005795478821</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>3.96534013748169</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>16</v>
       </c>
@@ -1270,8 +1622,17 @@
         <f aca="false">F31*2</f>
         <v>512</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="0" t="n">
+        <v>3.92397999763489</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>3.64270005226135</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>3.92397999763489</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>16</v>
       </c>
@@ -1288,8 +1649,17 @@
         <f aca="false">F32*2</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="n">
+        <v>3.89232993125916</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>3.61539998054504</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>3.89232993125916</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>16</v>
       </c>
@@ -1306,8 +1676,17 @@
         <f aca="false">F33*2</f>
         <v>2048</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="0" t="n">
+        <v>3.90987992286682</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>3.61475601196289</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>3.90987992286682</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>16</v>
       </c>
@@ -1324,8 +1703,17 @@
         <f aca="false">F34*2</f>
         <v>4096</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="0" t="n">
+        <v>4.71823000907898</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>3.7198920249939</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>4.71823000907898</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>16</v>
       </c>
@@ -1342,8 +1730,17 @@
         <f aca="false">F35*2</f>
         <v>8192</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="0" t="n">
+        <v>4.58207011222839</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>3.63034205436707</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>4.58207011222839</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>16</v>
       </c>
@@ -1360,8 +1757,17 @@
         <f aca="false">F36*2</f>
         <v>16384</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="0" t="n">
+        <v>4.5218198299408</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>3.6222499370575</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>4.5218198299408</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>16</v>
       </c>
@@ -1378,8 +1784,17 @@
         <f aca="false">F37*2</f>
         <v>32768</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="0" t="n">
+        <v>4.26800990104675</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>3.54289202690124</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>4.26800990104675</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>16</v>
       </c>
@@ -1396,8 +1811,17 @@
         <f aca="false">F38*2</f>
         <v>65536</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="0" t="n">
+        <v>4.12046003341675</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>3.58147406578064</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>4.12046003341675</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>16</v>
       </c>
@@ -1414,8 +1838,17 @@
         <f aca="false">F39*2</f>
         <v>131072</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0" t="n">
+        <v>4.24796986579895</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>3.68251996040344</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>4.24796986579895</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>16</v>
       </c>
@@ -1432,8 +1865,17 @@
         <f aca="false">F40*2</f>
         <v>262144</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0" t="n">
+        <v>4.68279004096985</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>3.94262399673462</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>4.68279004096985</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>16</v>
       </c>
@@ -1449,6 +1891,15 @@
       <c r="F42" s="0" t="n">
         <f aca="false">F41*2</f>
         <v>524288</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>4.60859990119934</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>4.2555579662323</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>4.60859990119934</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,13 +1941,17 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,7 +1986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>17</v>
       </c>
@@ -1550,8 +2005,17 @@
       <c r="G2" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>0.023921728134155</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1.20147931575775</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>4.0210018157959</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>17</v>
       </c>
@@ -1570,8 +2034,17 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>0.023354768753052</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.096855449676514</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.389429807662964</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>17</v>
       </c>
@@ -1590,8 +2063,17 @@
       <c r="G4" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>0.023509502410889</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.096988296508789</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.390338182449341</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
@@ -1609,6 +2091,15 @@
       </c>
       <c r="G5" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.020853757858276</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.021093893051148</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.021468639373779</v>
       </c>
     </row>
   </sheetData>
@@ -1630,12 +2121,16 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,7 +2162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -1683,8 +2178,17 @@
       <c r="F2" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0" t="n">
+        <v>-0.00453996658325195</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0.00564002990722656</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.0131399631500244</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
@@ -1701,8 +2205,17 @@
       <c r="F3" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <v>-0.0047299861907959</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.0294060230255127</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.112600088119507</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
@@ -1719,8 +2232,17 @@
       <c r="F4" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>-0.0047299861907959</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.0115880012512207</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.0217099189758301</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -1737,8 +2259,17 @@
       <c r="F5" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>0.482379913330078</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.59369387626648</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.768449783325195</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
@@ -1755,8 +2286,17 @@
       <c r="F6" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>2.2589099407196</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2.26663599014282</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>2.27320003509521</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
@@ -1773,8 +2313,17 @@
       <c r="F7" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>0.511080026626587</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.600830030441284</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.692280054092407</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -1791,8 +2340,17 @@
       <c r="F8" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="n">
+        <v>0.487919807434082</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.627553939819336</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.911959886550903</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
@@ -1809,8 +2367,17 @@
       <c r="F9" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="n">
+        <v>2.71451997756958</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2.7335159778595</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>2.78442001342773</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
@@ -1827,8 +2394,17 @@
       <c r="F10" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="n">
+        <v>0.42861008644104</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.540923976898193</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.596970081329346</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
@@ -1845,8 +2421,17 @@
       <c r="F11" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="n">
+        <v>0.107069969177246</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.300014019012451</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.470510005950928</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>14</v>
       </c>
@@ -1863,8 +2448,17 @@
       <c r="F12" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <v>0.0738799571990967</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.0866079330444336</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.596479892730713</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>16</v>
       </c>
@@ -1880,8 +2474,17 @@
       <c r="F13" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="n">
+        <v>0.0320301055908203</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.0718220233917236</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.180789947509766</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>16</v>
       </c>
@@ -1898,8 +2501,17 @@
       <c r="F14" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="n">
+        <v>0.0492699146270752</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.116214036941528</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.181079864501953</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>16</v>
       </c>
@@ -1916,8 +2528,17 @@
       <c r="F15" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="0" t="n">
+        <v>0.0492699146270752</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.0545280456542969</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.0587000846862793</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>16</v>
       </c>
@@ -1934,8 +2555,17 @@
       <c r="F16" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>0.519579887390137</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.720029973983765</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.936589956283569</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>16</v>
       </c>
@@ -1952,8 +2582,17 @@
       <c r="F17" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>2.34789991378784</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>2.36185402870178</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>2.38102006912231</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>16</v>
       </c>
@@ -1970,8 +2609,17 @@
       <c r="F18" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>0.547809839248657</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.707963991165161</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0.822309970855713</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>16</v>
       </c>
@@ -1988,8 +2636,17 @@
       <c r="F19" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>0.524780035018921</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.833135986328125</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1.08378982543945</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>16</v>
       </c>
@@ -2006,8 +2663,17 @@
       <c r="F20" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>2.95243000984192</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3.10746202468872</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>3.49880003929138</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>16</v>
       </c>
@@ -2024,8 +2690,17 @@
       <c r="F21" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>0.707839965820313</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.861243963241577</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1.01678991317749</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>16</v>
       </c>
@@ -2042,8 +2717,17 @@
       <c r="F22" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="n">
+        <v>0.213319778442383</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.426457977294922</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0.538520097732544</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>16</v>
       </c>
@@ -2059,6 +2743,15 @@
       </c>
       <c r="F23" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0.111359834671021</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.250009965896606</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.427639961242676</v>
       </c>
     </row>
   </sheetData>
@@ -2077,15 +2770,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,6 +2834,9 @@
       <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <v>0.030691623687744</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -2160,6 +2858,9 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>0.030956983566284</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
@@ -2181,6 +2882,9 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <v>1.19952988624573</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
@@ -2202,6 +2906,9 @@
       <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>0.54817008972168</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
@@ -2223,6 +2930,9 @@
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <v>0.030476808547974</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -2244,6 +2954,9 @@
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <v>0.030541658401489</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
@@ -2265,6 +2978,9 @@
       <c r="G8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>0.030620098114014</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -2286,6 +3002,9 @@
       <c r="G9" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>0.030864238739014</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
@@ -2307,6 +3026,9 @@
       <c r="G10" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>0.111570358276367</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -2328,6 +3050,9 @@
       <c r="G11" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>0.061688184738159</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
@@ -2349,8 +3074,35 @@
       <c r="G12" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
+      <c r="I12" s="0" t="n">
+        <v>0.030667781829834</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:P14"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2366,15 +3118,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,16 +3151,16 @@
         <v>10</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -2422,8 +3176,20 @@
       <c r="F2" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
@@ -2440,8 +3206,20 @@
       <c r="F3" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
@@ -2458,8 +3236,20 @@
       <c r="F4" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -2476,8 +3266,20 @@
       <c r="F5" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
@@ -2494,8 +3296,20 @@
       <c r="F6" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
@@ -2512,8 +3326,20 @@
       <c r="F7" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -2530,8 +3356,20 @@
       <c r="F8" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
@@ -2548,8 +3386,20 @@
       <c r="F9" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
@@ -2566,8 +3416,20 @@
       <c r="F10" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
@@ -2584,8 +3446,20 @@
       <c r="F11" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>14</v>
       </c>
@@ -2602,8 +3476,20 @@
       <c r="F12" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>16</v>
       </c>
@@ -2619,8 +3505,20 @@
       <c r="F13" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>16</v>
       </c>
@@ -2637,8 +3535,20 @@
       <c r="F14" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>16</v>
       </c>
@@ -2655,8 +3565,20 @@
       <c r="F15" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>16</v>
       </c>
@@ -2673,8 +3595,20 @@
       <c r="F16" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>16</v>
       </c>
@@ -2691,8 +3625,20 @@
       <c r="F17" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>16</v>
       </c>
@@ -2709,8 +3655,20 @@
       <c r="F18" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>16</v>
       </c>
@@ -2727,8 +3685,20 @@
       <c r="F19" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>16</v>
       </c>
@@ -2745,8 +3715,20 @@
       <c r="F20" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>16</v>
       </c>
@@ -2763,8 +3745,20 @@
       <c r="F21" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>16</v>
       </c>
@@ -2781,8 +3775,20 @@
       <c r="F22" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>16</v>
       </c>
@@ -2798,6 +3804,18 @@
       </c>
       <c r="F23" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2819,7 +3837,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2827,8 +3845,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.53"/>
   </cols>
@@ -2856,16 +3874,16 @@
         <v>8</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>17</v>
       </c>
@@ -2884,8 +3902,17 @@
       <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>17</v>
       </c>
@@ -2905,8 +3932,17 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>17</v>
       </c>
@@ -2926,8 +3962,17 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
@@ -2947,8 +3992,17 @@
       <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
@@ -2968,8 +4022,17 @@
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>17</v>
       </c>
@@ -2989,8 +4052,17 @@
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>17</v>
       </c>
@@ -3010,8 +4082,17 @@
       <c r="G8" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
@@ -3031,8 +4112,17 @@
       <c r="G9" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>17</v>
       </c>
@@ -3052,8 +4142,17 @@
       <c r="G10" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>17</v>
       </c>
@@ -3073,8 +4172,17 @@
       <c r="G11" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>17</v>
       </c>
@@ -3093,6 +4201,15 @@
       </c>
       <c r="G12" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3114,13 +4231,13 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -3144,7 +4261,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>